<commit_message>
Added TC for NGC1928
</commit_message>
<xml_diff>
--- a/Test Data/TC_149_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_Accessories.xlsx
+++ b/Test Data/TC_149_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_Accessories.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhasip\Desktop\NGConsys Automation_01_02_2019\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5449F99-1334-40FD-AB24-B0003CAEA3F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="6" r:id="rId1"/>
@@ -138,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -553,11 +554,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,10 +707,10 @@
         <v>14</v>
       </c>
       <c r="F8" s="15">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="G8" s="15">
-        <v>0.33600000000000002</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>33</v>
@@ -742,7 +743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>